<commit_message>
Adding new common methods
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/SampleTestData.xlsx
+++ b/src/test/resources/testdata/SampleTestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrrudenko/eclipse-workspace/SyntaxHrms/src/test/resources/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrrudenko/eclipse-workspace/CucumberFramework/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D224AD-A717-1B4D-8853-ADFCA95DB438}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6F02C6-B7EE-1547-995A-050800B43A9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16260" xr2:uid="{10507B24-6705-124A-9C9F-1E37CC554E52}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>MiddleName</t>
   </si>
@@ -36,24 +36,12 @@
     <t>FirstName</t>
   </si>
   <si>
-    <t>John</t>
-  </si>
-  <si>
     <t>Doe</t>
   </si>
   <si>
-    <t>Jane</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
     <t>Smith</t>
   </si>
   <si>
-    <t>Jack</t>
-  </si>
-  <si>
     <t>Rose</t>
   </si>
   <si>
@@ -63,24 +51,9 @@
     <t>Kate</t>
   </si>
   <si>
-    <t>Helem</t>
-  </si>
-  <si>
     <t>Niko</t>
   </si>
   <si>
-    <t>Ame</t>
-  </si>
-  <si>
-    <t>Byu</t>
-  </si>
-  <si>
-    <t>Cow</t>
-  </si>
-  <si>
-    <t>Due</t>
-  </si>
-  <si>
     <t>Eal</t>
   </si>
   <si>
@@ -88,9 +61,6 @@
   </si>
   <si>
     <t>Ginger</t>
-  </si>
-  <si>
-    <t>Hel</t>
   </si>
   <si>
     <t>Iel</t>
@@ -445,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECAC0E78-C0C1-944E-82B9-4E108179021A}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -473,21 +443,21 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -495,13 +465,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -509,65 +479,10 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>